<commit_message>
added zin absoprtion data
</commit_message>
<xml_diff>
--- a/tables/gdd_approach/TableS1_global_inadequacies.xlsx
+++ b/tables/gdd_approach/TableS1_global_inadequacies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/global_intake_inadequacies/tables/gdd_approach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420B24D2-95C7-8745-A5A9-50237ABE9DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31834384-A488-C141-888F-1FD915A8B926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="3760" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -554,15 +554,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color indexed="64"/>
@@ -617,11 +608,11 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -981,7 +972,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F17" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,32 +986,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1037,10 +1028,10 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>5.0636951699998596</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0.668687332273737</v>
       </c>
     </row>
@@ -1057,10 +1048,10 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>4.10965250783598</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0.54270102756540695</v>
       </c>
     </row>
@@ -1077,10 +1068,10 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>4.04961523791704</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0.53477279324021698</v>
       </c>
     </row>
@@ -1097,10 +1088,10 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>4.03203737431779</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>0.53245154476007694</v>
       </c>
     </row>
@@ -1117,10 +1108,10 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>3.88023354606716</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>0.51240505824500104</v>
       </c>
     </row>
@@ -1137,10 +1128,10 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>3.6258507520371501</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>0.47881248479704802</v>
       </c>
     </row>
@@ -1157,10 +1148,10 @@
       <c r="D9" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>2.9641747525236601</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>0.39143472130812901</v>
       </c>
     </row>
@@ -1177,10 +1168,10 @@
       <c r="D10" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>2.2348684696742498</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>0.29512602650787201</v>
       </c>
     </row>
@@ -1197,10 +1188,10 @@
       <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="2">
         <v>1.67320704548258</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>0.220955708829803</v>
       </c>
     </row>
@@ -1217,10 +1208,10 @@
       <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="2">
         <v>5.4700560129126403</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>0.72234939897904005</v>
       </c>
     </row>
@@ -1237,10 +1228,10 @@
       <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="2">
         <v>3.7818351536102899</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
         <v>0.49941103780280999</v>
       </c>
     </row>
@@ -1257,10 +1248,10 @@
       <c r="D14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="2">
         <v>3.35915893807277</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
         <v>0.44359444112893198</v>
       </c>
     </row>
@@ -1277,10 +1268,10 @@
       <c r="D15" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="2">
         <v>3.3588247903917798</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
         <v>0.44355031518653398</v>
       </c>
     </row>
@@ -1297,10 +1288,10 @@
       <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2">
         <v>1.99422478845216</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
         <v>0.26334777449572899</v>
       </c>
     </row>
@@ -1317,10 +1308,10 @@
       <c r="D17" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="2">
         <v>1.0086494819607199</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="3">
         <v>0.13319741979879501</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated iron ARs figs and shiny app
</commit_message>
<xml_diff>
--- a/tables/gdd_approach/TableS1_global_inadequacies.xlsx
+++ b/tables/gdd_approach/TableS1_global_inadequacies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/nutrition/global_intake_inadequacies/tables/gdd_approach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31834384-A488-C141-888F-1FD915A8B926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEC964E-82EE-5849-A874-1BEC46A3FAF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="3760" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18960" yWindow="4380" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableS1_global_inadequacies" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
     <t>µg RAE</t>
   </si>
   <si>
-    <t>µg</t>
+    <t>ug</t>
   </si>
 </sst>
 </file>
@@ -117,7 +117,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -610,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -969,20 +969,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="A1:F17"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1220,19 +1220,19 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2">
-        <v>3.7818351536102899</v>
+        <v>4.7672493213966503</v>
       </c>
       <c r="F13" s="3">
-        <v>0.49941103780280999</v>
+        <v>0.62954011329410098</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1240,19 +1240,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E14" s="2">
-        <v>3.35915893807277</v>
+        <v>3.7818351536102899</v>
       </c>
       <c r="F14" s="3">
-        <v>0.44359444112893198</v>
+        <v>0.49941103780280999</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1260,19 +1260,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2">
-        <v>3.3588247903917798</v>
+        <v>3.4799951323483098</v>
       </c>
       <c r="F15" s="3">
-        <v>0.44355031518653398</v>
+        <v>0.45955149021650998</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1280,19 +1280,19 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E16" s="2">
-        <v>1.99422478845216</v>
+        <v>3.3588247903917798</v>
       </c>
       <c r="F16" s="3">
-        <v>0.26334777449572899</v>
+        <v>0.44355031518653398</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1314,6 +1314,10 @@
       <c r="F17" s="3">
         <v>0.13319741979879501</v>
       </c>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E34" s="2"/>
+      <c r="F34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>